<commit_message>
Vikor & ANOVA & plots done
</commit_message>
<xml_diff>
--- a/Numerical Experiments/Numerical Results.xlsx
+++ b/Numerical Experiments/Numerical Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarzaminDigital\Desktop\PAPER\MATLAB\Numerical Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E860D0F9-8DD6-4DC8-8A5D-0E3662235DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D78D57C-CA01-4338-96CE-3602CE028FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D6129A20-1F81-494B-BF6B-C0ED5DF90618}"/>
   </bookViews>
@@ -128,12 +128,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="P41" authorId="0" shapeId="0" xr:uid="{28213FEE-10AF-4DDC-B469-C836533B4192}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SarzaminDigital:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+it was zero, but changed because 0/ln(0) equals infinity</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="31">
   <si>
     <t>NSGA-II</t>
   </si>
@@ -293,7 +317,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +357,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -473,6 +503,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,9 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,9 +836,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA82E70-FE4C-4668-AB26-ACA18349451D}">
-  <dimension ref="A1:AO29"/>
+  <dimension ref="A1:AO31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:D31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -842,48 +878,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="I1" s="31" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="I1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="P1" s="31" t="s">
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="P1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="W1" s="31" t="s">
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="W1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AD1" s="31" t="s">
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AD1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AK1" s="31" t="s">
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AK1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="34"/>
+      <c r="AO1" s="34"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -3982,6 +4018,139 @@
       </c>
       <c r="AO29" s="3">
         <f t="shared" ref="AO29" si="77">SUM(AO21:AO28)/8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="32">
+        <f>SUM(B3:B10,B12:B19,B21:B28)/24</f>
+        <v>3.375</v>
+      </c>
+      <c r="C31" s="32">
+        <f t="shared" ref="C31:AO31" si="78">SUM(C3:C10,C12:C19,C21:C28)/24</f>
+        <v>14.208333333333334</v>
+      </c>
+      <c r="D31" s="32">
+        <f t="shared" si="78"/>
+        <v>18</v>
+      </c>
+      <c r="E31" s="32">
+        <f t="shared" si="78"/>
+        <v>22.583333333333332</v>
+      </c>
+      <c r="F31" s="32">
+        <f t="shared" si="78"/>
+        <v>21.416666666666668</v>
+      </c>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32">
+        <f t="shared" si="78"/>
+        <v>1.0838745833333334</v>
+      </c>
+      <c r="J31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.90881500000000026</v>
+      </c>
+      <c r="K31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.95703791666666704</v>
+      </c>
+      <c r="L31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.91374583333333337</v>
+      </c>
+      <c r="M31" s="32">
+        <f t="shared" si="78"/>
+        <v>1.0984029166666667</v>
+      </c>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32">
+        <f t="shared" si="78"/>
+        <v>94.668854166666677</v>
+      </c>
+      <c r="Q31" s="32">
+        <f t="shared" si="78"/>
+        <v>120.17523749999999</v>
+      </c>
+      <c r="R31" s="32">
+        <f t="shared" si="78"/>
+        <v>98.892837500000027</v>
+      </c>
+      <c r="S31" s="32">
+        <f t="shared" si="78"/>
+        <v>133.35043333333331</v>
+      </c>
+      <c r="T31" s="32">
+        <f t="shared" si="78"/>
+        <v>197.40518208333333</v>
+      </c>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.3261208333333333</v>
+      </c>
+      <c r="X31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.2563758333333333</v>
+      </c>
+      <c r="Y31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.2377470833333333</v>
+      </c>
+      <c r="Z31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.24596291666666667</v>
+      </c>
+      <c r="AA31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.17683670833333331</v>
+      </c>
+      <c r="AB31" s="32"/>
+      <c r="AC31" s="32"/>
+      <c r="AD31" s="32">
+        <f t="shared" si="78"/>
+        <v>18.154199999999999</v>
+      </c>
+      <c r="AE31" s="32">
+        <f t="shared" si="78"/>
+        <v>19.350054166666663</v>
+      </c>
+      <c r="AF31" s="32">
+        <f t="shared" si="78"/>
+        <v>19.230904166666665</v>
+      </c>
+      <c r="AG31" s="32">
+        <f t="shared" si="78"/>
+        <v>19.399091666666667</v>
+      </c>
+      <c r="AH31" s="32">
+        <f t="shared" si="78"/>
+        <v>17.080270833333334</v>
+      </c>
+      <c r="AI31" s="32"/>
+      <c r="AJ31" s="32"/>
+      <c r="AK31" s="32">
+        <f t="shared" si="78"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AL31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.61321666666666652</v>
+      </c>
+      <c r="AM31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.58569583333333342</v>
+      </c>
+      <c r="AN31" s="32">
+        <f t="shared" si="78"/>
+        <v>0.75784583333333322</v>
+      </c>
+      <c r="AO31" s="32">
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
     </row>
@@ -4001,10 +4170,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D37A0FC-DBA9-4B44-8E5C-722A81CC8EDB}">
-  <dimension ref="B2:Y34"/>
+  <dimension ref="B2:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4467,7 +4636,7 @@
         <f t="shared" si="13"/>
         <v>2.6747624999999999</v>
       </c>
-      <c r="Q9" s="35" t="s">
+      <c r="Q9" s="31" t="s">
         <v>30</v>
       </c>
       <c r="R9" s="25">
@@ -4683,27 +4852,27 @@
         <v>3.5692105620078948E-2</v>
       </c>
       <c r="R15">
-        <f>K15*LN(K15)</f>
+        <f t="shared" ref="R15:W19" si="18">K15*LN(K15)</f>
         <v>-0.12174321617155119</v>
       </c>
       <c r="S15">
-        <f>L15*LN(L15)</f>
+        <f t="shared" si="18"/>
         <v>-0.32898905061240374</v>
       </c>
       <c r="T15">
-        <f>M15*LN(M15)</f>
+        <f t="shared" si="18"/>
         <v>-0.30606801092350638</v>
       </c>
       <c r="U15">
-        <f>N15*LN(N15)</f>
+        <f t="shared" si="18"/>
         <v>-0.36206423687173878</v>
       </c>
       <c r="V15">
-        <f>O15*LN(O15)</f>
+        <f t="shared" si="18"/>
         <v>-0.31334629266012487</v>
       </c>
       <c r="W15">
-        <f>P15*LN(P15)</f>
+        <f t="shared" si="18"/>
         <v>-0.11895556853026525</v>
       </c>
       <c r="X15" s="21"/>
@@ -4758,27 +4927,27 @@
         <v>0.28001170701064337</v>
       </c>
       <c r="R16">
-        <f>K16*LN(K16)</f>
+        <f t="shared" si="18"/>
         <v>-0.3063805565426127</v>
       </c>
       <c r="S16">
-        <f>L16*LN(L16)</f>
+        <f t="shared" si="18"/>
         <v>-0.30866855597875265</v>
       </c>
       <c r="T16">
-        <f>M16*LN(M16)</f>
+        <f t="shared" si="18"/>
         <v>-0.32701532046555215</v>
       </c>
       <c r="U16">
-        <f>N16*LN(N16)</f>
+        <f t="shared" si="18"/>
         <v>-0.32114308073332121</v>
       </c>
       <c r="V16">
-        <f>O16*LN(O16)</f>
+        <f t="shared" si="18"/>
         <v>-0.32673708244047844</v>
       </c>
       <c r="W16">
-        <f>P16*LN(P16)</f>
+        <f t="shared" si="18"/>
         <v>-0.35643358459494445</v>
       </c>
       <c r="X16" s="21"/>
@@ -4833,27 +5002,27 @@
         <v>0.32075067636540144</v>
       </c>
       <c r="R17">
-        <f>K17*LN(K17)</f>
+        <f t="shared" si="18"/>
         <v>-0.3491796401980361</v>
       </c>
       <c r="S17">
-        <f>L17*LN(L17)</f>
+        <f t="shared" si="18"/>
         <v>-0.31891591222573867</v>
       </c>
       <c r="T17">
-        <f>M17*LN(M17)</f>
+        <f t="shared" si="18"/>
         <v>-0.30443130630633813</v>
       </c>
       <c r="U17">
-        <f>N17*LN(N17)</f>
+        <f t="shared" si="18"/>
         <v>-0.30071596971932962</v>
       </c>
       <c r="V17">
-        <f>O17*LN(O17)</f>
+        <f t="shared" si="18"/>
         <v>-0.32636381986476215</v>
       </c>
       <c r="W17">
-        <f>P17*LN(P17)</f>
+        <f t="shared" si="18"/>
         <v>-0.36472276083669519</v>
       </c>
       <c r="X17" s="21"/>
@@ -4908,27 +5077,27 @@
         <v>0.36354551100387611</v>
       </c>
       <c r="R18">
-        <f>K18*LN(K18)</f>
+        <f t="shared" si="18"/>
         <v>-0.35180546087455578</v>
       </c>
       <c r="S18">
-        <f>L18*LN(L18)</f>
+        <f t="shared" si="18"/>
         <v>-0.3156714321496023</v>
       </c>
       <c r="T18">
-        <f>M18*LN(M18)</f>
+        <f t="shared" si="18"/>
         <v>-0.31557230411110504</v>
       </c>
       <c r="U18">
-        <f>N18*LN(N18)</f>
+        <f t="shared" si="18"/>
         <v>-0.30133463054030024</v>
       </c>
       <c r="V18">
-        <f>O18*LN(O18)</f>
+        <f t="shared" si="18"/>
         <v>-0.32736275405961762</v>
       </c>
       <c r="W18">
-        <f>P18*LN(P18)</f>
+        <f t="shared" si="18"/>
         <v>-0.36785381165015596</v>
       </c>
       <c r="X18" s="21"/>
@@ -4982,27 +5151,27 @@
         <v>1E-4</v>
       </c>
       <c r="R19">
-        <f>K19*LN(K19)</f>
+        <f t="shared" si="18"/>
         <v>-0.35180546087455578</v>
       </c>
       <c r="S19">
-        <f>L19*LN(L19)</f>
+        <f t="shared" si="18"/>
         <v>-0.33428746170142748</v>
       </c>
       <c r="T19">
-        <f>M19*LN(M19)</f>
+        <f t="shared" si="18"/>
         <v>-0.34680413761084683</v>
       </c>
       <c r="U19">
-        <f>N19*LN(N19)</f>
+        <f t="shared" si="18"/>
         <v>-0.2909539778176522</v>
       </c>
       <c r="V19">
-        <f>O19*LN(O19)</f>
+        <f t="shared" si="18"/>
         <v>-0.31429440120760038</v>
       </c>
       <c r="W19">
-        <f>P19*LN(P19)</f>
+        <f t="shared" si="18"/>
         <v>-9.2103403719761819E-4</v>
       </c>
       <c r="X19" s="21"/>
@@ -5016,26 +5185,26 @@
         <v>98.25</v>
       </c>
       <c r="D20" s="20">
-        <f t="shared" ref="D20:H20" si="18">SUM(D15:D19)</f>
+        <f t="shared" ref="D20:H20" si="19">SUM(D15:D19)</f>
         <v>4.84504</v>
       </c>
       <c r="E20" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>598.23566249999999</v>
       </c>
       <c r="F20" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.18781925</v>
       </c>
       <c r="G20" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>80.916412500000007</v>
       </c>
       <c r="H20" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.7510875000000001</v>
       </c>
-      <c r="Q20" s="35" t="s">
+      <c r="Q20" s="31" t="s">
         <v>30</v>
       </c>
       <c r="R20" s="25">
@@ -5043,23 +5212,23 @@
         <v>-1.4809143346613116</v>
       </c>
       <c r="S20" s="25">
-        <f t="shared" ref="S20:W20" si="19">SUM(S15:S19)</f>
+        <f t="shared" ref="S20:W20" si="20">SUM(S15:S19)</f>
         <v>-1.6065324126679248</v>
       </c>
       <c r="T20" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-1.5998910794173486</v>
       </c>
       <c r="U20" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-1.5762118956823419</v>
       </c>
       <c r="V20" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-1.6081043502325834</v>
       </c>
       <c r="W20" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-1.2088867596492585</v>
       </c>
       <c r="X20" s="21"/>
@@ -5073,23 +5242,23 @@
         <v>0.92014381121517719</v>
       </c>
       <c r="S21" s="21">
-        <f t="shared" ref="S21:W21" si="20">S20*(-$S$2)</f>
+        <f t="shared" ref="S21:W21" si="21">S20*(-$S$2)</f>
         <v>0.99819471149292038</v>
       </c>
       <c r="T21" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.99406821913228516</v>
       </c>
       <c r="U21" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.9793555150558696</v>
       </c>
       <c r="V21" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.99917141121678932</v>
       </c>
       <c r="W21" s="21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.75112357569665322</v>
       </c>
       <c r="X21" s="21"/>
@@ -5103,27 +5272,27 @@
         <v>7.9856188784822812E-2</v>
       </c>
       <c r="S22">
-        <f t="shared" ref="S22:W22" si="21">$U$2-S21</f>
+        <f t="shared" ref="S22:W22" si="22">$U$2-S21</f>
         <v>1.8052885070796165E-3</v>
       </c>
       <c r="T22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5.931780867714842E-3</v>
       </c>
       <c r="U22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2.0644484944130403E-2</v>
       </c>
       <c r="V22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>8.2858878321068197E-4</v>
       </c>
       <c r="W22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.24887642430334678</v>
       </c>
       <c r="X22" s="21">
-        <f t="shared" ref="X12:Y33" si="22">SUM(R22:W22)</f>
+        <f t="shared" ref="X22:X33" si="23">SUM(R22:W22)</f>
         <v>0.35794275619030513</v>
       </c>
       <c r="Y22">
@@ -5139,23 +5308,23 @@
         <v>0.22309765291734576</v>
       </c>
       <c r="S23" s="30">
-        <f t="shared" ref="S23:W23" si="23">S22/$Y$22</f>
+        <f t="shared" ref="S23:W23" si="24">S22/$Y$22</f>
         <v>5.0435117790728814E-3</v>
       </c>
       <c r="T23" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.657187012484513E-2</v>
       </c>
       <c r="U23" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>5.7675381292405542E-2</v>
       </c>
       <c r="V23" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2.3148639520732513E-3</v>
       </c>
       <c r="W23" s="30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.69529671993425746</v>
       </c>
       <c r="X23" s="21"/>
@@ -5256,23 +5425,23 @@
         <v>-0.10933385000877538</v>
       </c>
       <c r="S26">
-        <f t="shared" ref="S20:S30" si="24">L26*LN(L26)</f>
+        <f t="shared" ref="S26:S30" si="25">L26*LN(L26)</f>
         <v>-0.33821775426533301</v>
       </c>
       <c r="T26">
-        <f t="shared" ref="T20:T30" si="25">M26*LN(M26)</f>
+        <f t="shared" ref="T26:T30" si="26">M26*LN(M26)</f>
         <v>-0.25674187200323467</v>
       </c>
       <c r="U26">
-        <f t="shared" ref="U20:U30" si="26">N26*LN(N26)</f>
+        <f t="shared" ref="U26:U30" si="27">N26*LN(N26)</f>
         <v>-0.34657271133750456</v>
       </c>
       <c r="V26">
-        <f t="shared" ref="V20:V30" si="27">O26*LN(O26)</f>
+        <f t="shared" ref="V26:V30" si="28">O26*LN(O26)</f>
         <v>-0.32034887225018777</v>
       </c>
       <c r="W26">
-        <f t="shared" ref="W20:W30" si="28">P26*LN(P26)</f>
+        <f t="shared" ref="W26:W30" si="29">P26*LN(P26)</f>
         <v>-9.2103403719761819E-4</v>
       </c>
       <c r="X26" s="21"/>
@@ -5327,27 +5496,27 @@
         <v>0.27435207161858638</v>
       </c>
       <c r="R27">
-        <f t="shared" ref="R20:R30" si="29">K27*LN(K27)</f>
+        <f t="shared" ref="R27:R30" si="30">K27*LN(K27)</f>
         <v>-0.30349188716548814</v>
       </c>
       <c r="S27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>-0.3002723611369108</v>
       </c>
       <c r="T27">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>-0.30325705625867883</v>
       </c>
       <c r="U27">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>-0.32951399525395808</v>
       </c>
       <c r="V27">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>-0.32610100265444653</v>
       </c>
       <c r="W27">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.35483134905892277</v>
       </c>
       <c r="X27" s="21"/>
@@ -5402,27 +5571,27 @@
         <v>0.20437421348583076</v>
       </c>
       <c r="R28">
+        <f t="shared" si="30"/>
+        <v>-0.32173897172598009</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="25"/>
+        <v>-0.31303296323832336</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="26"/>
+        <v>-0.2693632577532995</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="27"/>
+        <v>-0.32583527132465495</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="28"/>
+        <v>-0.32484234140474355</v>
+      </c>
+      <c r="W28">
         <f t="shared" si="29"/>
-        <v>-0.32173897172598009</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="24"/>
-        <v>-0.31303296323832336</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="25"/>
-        <v>-0.2693632577532995</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="26"/>
-        <v>-0.32583527132465495</v>
-      </c>
-      <c r="V28">
-        <f t="shared" si="27"/>
-        <v>-0.32484234140474355</v>
-      </c>
-      <c r="W28">
-        <f t="shared" si="28"/>
         <v>-0.32450590462839635</v>
       </c>
       <c r="X28" s="21"/>
@@ -5477,27 +5646,27 @@
         <v>0.52127371489558283</v>
       </c>
       <c r="R29">
+        <f t="shared" si="30"/>
+        <v>-0.36449548683450528</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="25"/>
+        <v>-0.29874138527696326</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="26"/>
+        <v>-0.33116693092483024</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="27"/>
+        <v>-0.33180063301993057</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="28"/>
+        <v>-0.32594099471580135</v>
+      </c>
+      <c r="W29">
         <f t="shared" si="29"/>
-        <v>-0.36449548683450528</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="24"/>
-        <v>-0.29874138527696326</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="25"/>
-        <v>-0.33116693092483024</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="26"/>
-        <v>-0.33180063301993057</v>
-      </c>
-      <c r="V29">
-        <f t="shared" si="27"/>
-        <v>-0.32594099471580135</v>
-      </c>
-      <c r="W29">
-        <f t="shared" si="28"/>
         <v>-0.33959940535857958</v>
       </c>
       <c r="X29" s="21"/>
@@ -5551,27 +5720,27 @@
         <v>1E-4</v>
       </c>
       <c r="R30">
+        <f t="shared" si="30"/>
+        <v>-0.35545078182390111</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="25"/>
+        <v>-0.34569543715972478</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="26"/>
+        <v>-0.36764962543653879</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="27"/>
+        <v>-0.24596184338035479</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="28"/>
+        <v>-0.31119507708492017</v>
+      </c>
+      <c r="W30">
         <f t="shared" si="29"/>
-        <v>-0.35545078182390111</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="24"/>
-        <v>-0.34569543715972478</v>
-      </c>
-      <c r="T30">
-        <f t="shared" si="25"/>
-        <v>-0.36764962543653879</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="26"/>
-        <v>-0.24596184338035479</v>
-      </c>
-      <c r="V30">
-        <f t="shared" si="27"/>
-        <v>-0.31119507708492017</v>
-      </c>
-      <c r="W30">
-        <f t="shared" si="28"/>
         <v>-9.2103403719761819E-4</v>
       </c>
       <c r="X30" s="21"/>
@@ -5585,26 +5754,26 @@
         <v>102.625</v>
       </c>
       <c r="D31" s="20">
-        <f t="shared" ref="D31:H31" si="30">SUM(D26:D30)</f>
+        <f t="shared" ref="D31:H31" si="31">SUM(D26:D30)</f>
         <v>4.6022762500000001</v>
       </c>
       <c r="E31" s="20">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1123.30665</v>
       </c>
       <c r="F31" s="20">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.3322471249999999</v>
       </c>
       <c r="G31" s="20">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>153.12162499999999</v>
       </c>
       <c r="H31" s="20">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.5694250000000001</v>
       </c>
-      <c r="Q31" s="35" t="s">
+      <c r="Q31" s="31" t="s">
         <v>30</v>
       </c>
       <c r="R31" s="25">
@@ -5612,23 +5781,23 @@
         <v>-1.45451097755865</v>
       </c>
       <c r="S31" s="25">
-        <f t="shared" ref="S31:W31" si="31">SUM(S26:S30)</f>
+        <f t="shared" ref="S31:W31" si="32">SUM(S26:S30)</f>
         <v>-1.5959599010772549</v>
       </c>
       <c r="T31" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-1.528178742376582</v>
       </c>
       <c r="U31" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-1.579684454316403</v>
       </c>
       <c r="V31" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-1.6084282881100993</v>
       </c>
       <c r="W31" s="25">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-1.0207787271202939</v>
       </c>
       <c r="X31" s="21"/>
@@ -5642,28 +5811,28 @@
         <v>0.90373848305764093</v>
       </c>
       <c r="S32" s="21">
-        <f t="shared" ref="S32:W32" si="32">S31*(-$S$2)</f>
+        <f t="shared" ref="S32:W32" si="33">S31*(-$S$2)</f>
         <v>0.99162564069560077</v>
       </c>
       <c r="T32" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.94951083888994359</v>
       </c>
       <c r="U32" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.98151313704751841</v>
       </c>
       <c r="V32" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.99937268513671706</v>
       </c>
       <c r="W32" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.63424548361513178</v>
       </c>
       <c r="X32" s="21"/>
     </row>
-    <row r="33" spans="17:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q33" s="23" t="s">
         <v>28</v>
       </c>
@@ -5672,34 +5841,34 @@
         <v>9.6261516942359071E-2</v>
       </c>
       <c r="S33">
-        <f t="shared" ref="S33:W33" si="33">$U$2-S32</f>
+        <f t="shared" ref="S33:W33" si="34">$U$2-S32</f>
         <v>8.3743593043992259E-3</v>
       </c>
       <c r="T33">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5.0489161110056413E-2</v>
       </c>
       <c r="U33">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1.8486862952481586E-2</v>
       </c>
       <c r="V33">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6.2731486328293506E-4</v>
       </c>
       <c r="W33">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.36575451638486822</v>
       </c>
       <c r="X33" s="21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.53999373155744745</v>
       </c>
       <c r="Y33">
         <v>0.53999373155744745</v>
       </c>
     </row>
-    <row r="34" spans="17:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q34" s="29" t="s">
         <v>29</v>
       </c>
@@ -5708,24 +5877,582 @@
         <v>0.17826413774234387</v>
       </c>
       <c r="S34" s="30">
-        <f t="shared" ref="S34:W34" si="34">S33/$Y$33</f>
+        <f t="shared" ref="S34:W34" si="35">S33/$Y$33</f>
         <v>1.5508252809242687E-2</v>
       </c>
       <c r="T34" s="30">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>9.3499531863889984E-2</v>
       </c>
       <c r="U34" s="30">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.4235328804950865E-2</v>
       </c>
       <c r="V34" s="30">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.1617076766310534E-3</v>
       </c>
       <c r="W34" s="30">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.67733104110294151</v>
+      </c>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>3.375</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1.0838745833333334</v>
+      </c>
+      <c r="E37" s="1">
+        <v>94.668854166666677</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.3261208333333333</v>
+      </c>
+      <c r="G37" s="1">
+        <v>18.154199999999999</v>
+      </c>
+      <c r="H37" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K37" s="19">
+        <f>C37/$C$42</f>
+        <v>4.2408376963350779E-2</v>
+      </c>
+      <c r="L37" s="19">
+        <f>D37/$D$42</f>
+        <v>0.21844047064521877</v>
+      </c>
+      <c r="M37" s="19">
+        <f>E37/$E$42</f>
+        <v>0.14688898259927957</v>
+      </c>
+      <c r="N37" s="19">
+        <f>F37/$F$42</f>
+        <v>0.26235676074725339</v>
+      </c>
+      <c r="O37" s="19">
+        <f>G37/$G$42</f>
+        <v>0.19475720990358933</v>
+      </c>
+      <c r="P37" s="19">
+        <f>H37/$H$42</f>
+        <v>2.0849752513437667E-2</v>
+      </c>
+      <c r="R37" s="1">
+        <f>K37*LN(K37)</f>
+        <v>-0.13402783176744879</v>
+      </c>
+      <c r="S37" s="1">
+        <f t="shared" ref="S37:W37" si="36">L37*LN(L37)</f>
+        <v>-0.33230076320739443</v>
+      </c>
+      <c r="T37" s="1">
+        <f t="shared" si="36"/>
+        <v>-0.28174455504112877</v>
+      </c>
+      <c r="U37" s="1">
+        <f t="shared" si="36"/>
+        <v>-0.3510464687624939</v>
+      </c>
+      <c r="V37" s="1">
+        <f t="shared" si="36"/>
+        <v>-0.31862310187002668</v>
+      </c>
+      <c r="W37" s="1">
+        <f t="shared" si="36"/>
+        <v>-8.0697157358646576E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>14.208333333333334</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.90881500000000026</v>
+      </c>
+      <c r="E38" s="1">
+        <v>120.17523749999999</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.2563758333333333</v>
+      </c>
+      <c r="G38" s="1">
+        <v>19.350054166666663</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.61321666666666652</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" s="19">
+        <f t="shared" ref="K38:K41" si="37">C38/$C$42</f>
+        <v>0.17853403141361254</v>
+      </c>
+      <c r="L38" s="19">
+        <f t="shared" ref="L38:L41" si="38">D38/$D$42</f>
+        <v>0.18315954574643009</v>
+      </c>
+      <c r="M38" s="19">
+        <f t="shared" ref="M38:M41" si="39">E38/$E$42</f>
+        <v>0.18646489941585545</v>
+      </c>
+      <c r="N38" s="19">
+        <f t="shared" ref="N38:N41" si="40">F38/$F$42</f>
+        <v>0.20624850145179635</v>
+      </c>
+      <c r="O38" s="19">
+        <f t="shared" ref="O38:O41" si="41">G38/$G$42</f>
+        <v>0.20758626438969069</v>
+      </c>
+      <c r="P38" s="19">
+        <f t="shared" ref="P38:P40" si="42">H38/$H$42</f>
+        <v>0.30684997769076477</v>
+      </c>
+      <c r="R38" s="1">
+        <f t="shared" ref="R38:R41" si="43">K38*LN(K38)</f>
+        <v>-0.30760985912104244</v>
+      </c>
+      <c r="S38" s="1">
+        <f t="shared" ref="S38:S41" si="44">L38*LN(L38)</f>
+        <v>-0.31089458642413575</v>
+      </c>
+      <c r="T38" s="1">
+        <f t="shared" ref="T38:T41" si="45">M38*LN(M38)</f>
+        <v>-0.31317008546710984</v>
+      </c>
+      <c r="U38" s="1">
+        <f t="shared" ref="U38:U41" si="46">N38*LN(N38)</f>
+        <v>-0.32559904767479614</v>
+      </c>
+      <c r="V38" s="1">
+        <f t="shared" ref="V38:V41" si="47">O38*LN(O38)</f>
+        <v>-0.32636884653280995</v>
+      </c>
+      <c r="W38" s="1">
+        <f t="shared" ref="W38:W41" si="48">P38*LN(P38)</f>
+        <v>-0.36251143531080404</v>
+      </c>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="1">
+        <v>18</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.95703791666666704</v>
+      </c>
+      <c r="E39" s="1">
+        <v>98.892837500000027</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.2377470833333333</v>
+      </c>
+      <c r="G39" s="1">
+        <v>19.230904166666665</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.58569583333333342</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" s="19">
+        <f t="shared" si="37"/>
+        <v>0.22617801047120417</v>
+      </c>
+      <c r="L39" s="19">
+        <f t="shared" si="38"/>
+        <v>0.19287823162995385</v>
+      </c>
+      <c r="M39" s="19">
+        <f t="shared" si="39"/>
+        <v>0.1534429503198281</v>
+      </c>
+      <c r="N39" s="19">
+        <f t="shared" si="40"/>
+        <v>0.19126209761854315</v>
+      </c>
+      <c r="O39" s="19">
+        <f t="shared" si="41"/>
+        <v>0.20630803006595227</v>
+      </c>
+      <c r="P39" s="19">
+        <f t="shared" si="42"/>
+        <v>0.2930787161556393</v>
+      </c>
+      <c r="R39" s="1">
+        <f t="shared" si="43"/>
+        <v>-0.33619844343880428</v>
+      </c>
+      <c r="S39" s="1">
+        <f t="shared" si="44"/>
+        <v>-0.31741897543893044</v>
+      </c>
+      <c r="T39" s="1">
+        <f t="shared" si="45"/>
+        <v>-0.28761752314047356</v>
+      </c>
+      <c r="U39" s="1">
+        <f t="shared" si="46"/>
+        <v>-0.31636865401274455</v>
+      </c>
+      <c r="V39" s="1">
+        <f t="shared" si="47"/>
+        <v>-0.32563348671754261</v>
+      </c>
+      <c r="W39" s="1">
+        <f t="shared" si="48"/>
+        <v>-0.35969962615980527</v>
+      </c>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="1">
+        <v>22.583333333333332</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.91374583333333337</v>
+      </c>
+      <c r="E40" s="1">
+        <v>133.35043333333331</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.24596291666666667</v>
+      </c>
+      <c r="G40" s="1">
+        <v>19.399091666666667</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.75784583333333322</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K40" s="19">
+        <f t="shared" si="37"/>
+        <v>0.28376963350785334</v>
+      </c>
+      <c r="L40" s="19">
+        <f t="shared" si="38"/>
+        <v>0.18415328946048043</v>
+      </c>
+      <c r="M40" s="19">
+        <f t="shared" si="39"/>
+        <v>0.20690764300391531</v>
+      </c>
+      <c r="N40" s="19">
+        <f t="shared" si="40"/>
+        <v>0.19787154785863101</v>
+      </c>
+      <c r="O40" s="19">
+        <f t="shared" si="41"/>
+        <v>0.20811233585968927</v>
+      </c>
+      <c r="P40" s="19">
+        <f t="shared" si="42"/>
+        <v>0.3792215536401583</v>
+      </c>
+      <c r="R40" s="1">
+        <f t="shared" si="43"/>
+        <v>-0.35743410765641775</v>
+      </c>
+      <c r="S40" s="1">
+        <f t="shared" si="44"/>
+        <v>-0.31158493002869236</v>
+      </c>
+      <c r="T40" s="1">
+        <f t="shared" si="45"/>
+        <v>-0.32597942329442897</v>
+      </c>
+      <c r="U40" s="1">
+        <f t="shared" si="46"/>
+        <v>-0.32057905689333938</v>
+      </c>
+      <c r="V40" s="1">
+        <f t="shared" si="47"/>
+        <v>-0.32666920296019591</v>
+      </c>
+      <c r="W40" s="1">
+        <f t="shared" si="48"/>
+        <v>-0.36770636619074404</v>
+      </c>
+    </row>
+    <row r="41" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>21.416666666666668</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1.0984029166666667</v>
+      </c>
+      <c r="E41">
+        <v>197.40518208333333</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.17683670833333331</v>
+      </c>
+      <c r="G41">
+        <v>17.080270833333334</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K41" s="19">
+        <f t="shared" si="37"/>
+        <v>0.26910994764397905</v>
+      </c>
+      <c r="L41" s="19">
+        <f t="shared" si="38"/>
+        <v>0.22136846251791675</v>
+      </c>
+      <c r="M41" s="19">
+        <f t="shared" si="39"/>
+        <v>0.30629552466112148</v>
+      </c>
+      <c r="N41" s="19">
+        <f t="shared" si="40"/>
+        <v>0.14226109232377618</v>
+      </c>
+      <c r="O41" s="19">
+        <f t="shared" si="41"/>
+        <v>0.18323615978107849</v>
+      </c>
+      <c r="P41" s="24">
+        <v>1E-4</v>
+      </c>
+      <c r="R41" s="1">
+        <f t="shared" si="43"/>
+        <v>-0.35324320490625782</v>
+      </c>
+      <c r="S41" s="1">
+        <f t="shared" si="44"/>
+        <v>-0.33380741839460532</v>
+      </c>
+      <c r="T41" s="1">
+        <f t="shared" si="45"/>
+        <v>-0.3624103583422153</v>
+      </c>
+      <c r="U41" s="1">
+        <f t="shared" si="46"/>
+        <v>-0.27742210870205214</v>
+      </c>
+      <c r="V41" s="1">
+        <f t="shared" si="47"/>
+        <v>-0.31094800085223118</v>
+      </c>
+      <c r="W41" s="1">
+        <f t="shared" si="48"/>
+        <v>-9.2103403719761819E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B42" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="20">
+        <f>SUM(C37:C41)</f>
+        <v>79.583333333333343</v>
+      </c>
+      <c r="D42" s="20">
+        <f t="shared" ref="D42:H42" si="49">SUM(D37:D41)</f>
+        <v>4.9618762500000013</v>
+      </c>
+      <c r="E42" s="20">
+        <f t="shared" si="49"/>
+        <v>644.49254458333337</v>
+      </c>
+      <c r="F42" s="20">
+        <f t="shared" si="49"/>
+        <v>1.2430433749999998</v>
+      </c>
+      <c r="G42" s="20">
+        <f t="shared" si="49"/>
+        <v>93.214520833333324</v>
+      </c>
+      <c r="H42" s="20">
+        <f t="shared" si="49"/>
+        <v>1.9984249999999997</v>
+      </c>
+      <c r="Q42" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="R42" s="20">
+        <f>SUM(R37:R41)</f>
+        <v>-1.488513446889971</v>
+      </c>
+      <c r="S42" s="20">
+        <f t="shared" ref="S42:W42" si="50">SUM(S37:S41)</f>
+        <v>-1.6060066734937584</v>
+      </c>
+      <c r="T42" s="20">
+        <f t="shared" si="50"/>
+        <v>-1.5709219452853567</v>
+      </c>
+      <c r="U42" s="20">
+        <f t="shared" si="50"/>
+        <v>-1.591015336045426</v>
+      </c>
+      <c r="V42" s="20">
+        <f t="shared" si="50"/>
+        <v>-1.6082426389328062</v>
+      </c>
+      <c r="W42" s="20">
+        <f t="shared" si="50"/>
+        <v>-1.1715356190571977</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Q43" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="R43" s="2">
+        <f>R42*(-$S$2)</f>
+        <v>0.92486540511448245</v>
+      </c>
+      <c r="S43" s="2">
+        <f t="shared" ref="S43:W43" si="51">S42*(-$S$2)</f>
+        <v>0.99786805137754431</v>
+      </c>
+      <c r="T43" s="2">
+        <f t="shared" si="51"/>
+        <v>0.97606868407213521</v>
+      </c>
+      <c r="U43" s="2">
+        <f t="shared" si="51"/>
+        <v>0.98855340970512362</v>
+      </c>
+      <c r="V43" s="2">
+        <f t="shared" si="51"/>
+        <v>0.99925733481729262</v>
+      </c>
+      <c r="W43" s="2">
+        <f t="shared" si="51"/>
+        <v>0.72791600720115834</v>
+      </c>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Q44" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="R44">
+        <f>$U$2-R43</f>
+        <v>7.5134594885517547E-2</v>
+      </c>
+      <c r="S44">
+        <f t="shared" ref="S44:W44" si="52">$U$2-S43</f>
+        <v>2.1319486224556927E-3</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="52"/>
+        <v>2.3931315927864794E-2</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="52"/>
+        <v>1.144659029487638E-2</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="52"/>
+        <v>7.4266518270738047E-4</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="52"/>
+        <v>0.27208399279884166</v>
+      </c>
+      <c r="X44" s="21">
+        <f>SUM(R44:W44)</f>
+        <v>0.38547110771226345</v>
+      </c>
+      <c r="Y44">
+        <v>0.38547110771226345</v>
+      </c>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Q45" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="R45" s="30">
+        <f>R44/$Y$44</f>
+        <v>0.19491628135616867</v>
+      </c>
+      <c r="S45" s="30">
+        <f t="shared" ref="S45:W45" si="53">S44/$Y$44</f>
+        <v>5.5307611382565533E-3</v>
+      </c>
+      <c r="T45" s="30">
+        <f t="shared" si="53"/>
+        <v>6.2083293531115767E-2</v>
+      </c>
+      <c r="U45" s="30">
+        <f t="shared" si="53"/>
+        <v>2.9695066804904961E-2</v>
+      </c>
+      <c r="V45" s="30">
+        <f t="shared" si="53"/>
+        <v>1.9266429256268567E-3</v>
+      </c>
+      <c r="W45" s="30">
+        <f t="shared" si="53"/>
+        <v>0.70584795424392721</v>
       </c>
     </row>
   </sheetData>
@@ -5737,9 +6464,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B29720-46E5-4342-BBA4-B9C9D1D80DDF}">
-  <dimension ref="A2:R34"/>
+  <dimension ref="A2:R46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:J46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5810,14 +6539,14 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="34"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37"/>
       <c r="L3" s="11" t="s">
         <v>17</v>
       </c>
@@ -6069,14 +6798,14 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
       <c r="L15" s="11" t="s">
         <v>17</v>
       </c>
@@ -6289,14 +7018,14 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="37"/>
       <c r="L27" s="11" t="s">
         <v>17</v>
       </c>
@@ -6413,7 +7142,7 @@
         <v>0.32074999999999998</v>
       </c>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
@@ -6436,7 +7165,7 @@
         <v>0.81810000000000005</v>
       </c>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
         <v>1</v>
       </c>
@@ -6459,11 +7188,228 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="37"/>
+      <c r="L39" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1">
+        <v>3.375</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1.0838745833333334</v>
+      </c>
+      <c r="G42" s="1">
+        <v>94.668854166666677</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0.3261208333333333</v>
+      </c>
+      <c r="I42" s="1">
+        <v>18.154199999999999</v>
+      </c>
+      <c r="J42" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>14.208333333333334</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.90881500000000026</v>
+      </c>
+      <c r="G43" s="1">
+        <v>120.17523749999999</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.2563758333333333</v>
+      </c>
+      <c r="I43" s="1">
+        <v>19.350054166666663</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.61321666666666652</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1">
+        <v>18</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.95703791666666704</v>
+      </c>
+      <c r="G44" s="1">
+        <v>98.892837500000027</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.2377470833333333</v>
+      </c>
+      <c r="I44" s="1">
+        <v>19.230904166666665</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.58569583333333342</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="1">
+        <v>22.583333333333332</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.91374583333333337</v>
+      </c>
+      <c r="G45" s="1">
+        <v>133.35043333333331</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.24596291666666667</v>
+      </c>
+      <c r="I45" s="1">
+        <v>19.399091666666667</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.75784583333333322</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <v>21.416666666666668</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1.0984029166666667</v>
+      </c>
+      <c r="G46">
+        <v>197.40518208333333</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.17683670833333331</v>
+      </c>
+      <c r="I46">
+        <v>17.080270833333334</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="E3:J3"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>